<commit_message>
numerics and floats working! :D
</commit_message>
<xml_diff>
--- a/test/numeric_test.xlsx
+++ b/test/numeric_test.xlsx
@@ -90,7 +90,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -101,10 +101,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -124,16 +120,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -146,6 +145,15 @@
       <c r="C1" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="D1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -155,6 +163,15 @@
         <v>-5</v>
       </c>
       <c r="C2" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>-5</v>
       </c>
     </row>
@@ -165,8 +182,17 @@
       <c r="B3" s="1" t="n">
         <v>3147483647</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="1" t="n">
         <v>3147483647</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>5.1234567</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>5.1234567</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>5.1234567</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -179,8 +205,17 @@
       <c r="C4" s="1" t="n">
         <v>-3147483647</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="0" t="n">
+        <v>5.12345678987654</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>5.12345678987654</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>5.12345678987654</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>5.5</v>
       </c>
@@ -189,6 +224,15 @@
       </c>
       <c r="C5" s="0" t="n">
         <v>5.5</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>12345678987654300</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>12345678987654300</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>12345678987654300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>